<commit_message>
Update Muscle for Life Meal Plan Template.xlsx
</commit_message>
<xml_diff>
--- a/Fitness/Muscle for Life Meal Plan Template.xlsx
+++ b/Fitness/Muscle for Life Meal Plan Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/urban/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlynch\Desktop\IS362Mac\Fitness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CCEEAC-BC4E-5843-B0B3-4EA1628B5094}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CE1354-78CC-47E7-A64E-6DC1C0F3C01E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="18945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cut" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Meal</t>
   </si>
@@ -144,6 +143,12 @@
   </si>
   <si>
     <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Unsalted Whole Cashews</t>
+  </si>
+  <si>
+    <t>Vega Protein and Greens 1 scoop</t>
   </si>
 </sst>
 </file>
@@ -260,12 +265,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,19 +590,19 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,8 +623,8 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -639,8 +644,8 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
       <c r="B3" s="17" t="s">
         <v>18</v>
       </c>
@@ -658,8 +663,8 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -667,8 +672,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -676,36 +681,36 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
       <c r="B6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -727,8 +732,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -747,8 +752,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
       <c r="B14" s="17" t="s">
         <v>18</v>
       </c>
@@ -765,277 +770,306 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2">
+        <v>170</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" ref="C23:F23" si="1">SUM(C13:C22)</f>
-        <v>410</v>
+        <v>580</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="2">
-        <v>240</v>
-      </c>
-      <c r="D24" s="17">
-        <v>52</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
-      <c r="B25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2">
-        <v>170</v>
-      </c>
-      <c r="D25" s="2">
-        <v>3</v>
-      </c>
-      <c r="E25" s="2">
-        <v>35</v>
-      </c>
-      <c r="F25" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
       <c r="B30" s="6"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
       <c r="B31" s="6"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
       <c r="B32" s="6"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22"/>
       <c r="B33" s="6"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="7">
         <f t="shared" ref="C34:F34" si="2">SUM(C24:C33)</f>
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F34" s="7">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="20"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>110</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+      <c r="C36">
+        <v>550</v>
+      </c>
+      <c r="D36">
+        <v>31</v>
+      </c>
+      <c r="E36">
+        <v>66</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+      <c r="C37">
+        <v>140</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>18</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="7">
         <f t="shared" ref="C40:F40" si="3">SUM(C35:C39)</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="F40" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="9">
         <f t="shared" ref="C42:F42" si="4">SUM(C12+C23+C34+C40)</f>
-        <v>1230</v>
+        <v>1790</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E42" s="9">
         <f t="shared" si="4"/>
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="F42" s="9">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
         <v>12</v>
@@ -1053,16 +1087,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="13"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="17" t="s">
         <v>14</v>
       </c>
@@ -1098,9 +1132,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1111,7 +1145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -1139,13 +1173,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1166,8 +1200,8 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2"/>
@@ -1177,8 +1211,8 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1186,8 +1220,8 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1195,8 +1229,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1204,36 +1238,36 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
       <c r="B6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1255,8 +1289,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
@@ -1265,79 +1299,79 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -1359,8 +1393,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2"/>
@@ -1369,56 +1403,56 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
       <c r="B30" s="6"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
       <c r="B31" s="6"/>
       <c r="C31" s="2">
         <v>500</v>
@@ -1427,23 +1461,23 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
       <c r="B32" s="6"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22"/>
       <c r="B33" s="6"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>7</v>
@@ -1465,24 +1499,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="20"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>7</v>
@@ -1504,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>11</v>
@@ -1526,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
         <v>12</v>
@@ -1536,7 +1570,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="5"/>
@@ -1544,7 +1578,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="13"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -1573,13 +1607,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1600,8 +1634,8 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2"/>
@@ -1611,8 +1645,8 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1620,8 +1654,8 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1629,8 +1663,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1638,36 +1672,36 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
       <c r="B6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1689,8 +1723,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
@@ -1699,79 +1733,79 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -1793,8 +1827,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2"/>
@@ -1803,79 +1837,79 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
       <c r="B30" s="6"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
       <c r="B31" s="6"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
       <c r="B32" s="6"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22"/>
       <c r="B33" s="6"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>7</v>
@@ -1897,24 +1931,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="20"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>7</v>
@@ -1936,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>11</v>
@@ -1958,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
         <v>12</v>
@@ -1968,7 +2002,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="5"/>
@@ -1976,7 +2010,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="13"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2001,17 +2035,17 @@
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2031,8 +2065,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -2051,79 +2085,79 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
       <c r="B3" s="17"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
       <c r="B6" s="2"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
       <c r="B8" s="2"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
       <c r="B9" s="2"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
       <c r="B10" s="2"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="2"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -2145,8 +2179,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
@@ -2155,79 +2189,79 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="22"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -2249,8 +2283,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="2"/>
@@ -2259,79 +2293,79 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
       <c r="B28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
       <c r="B29" s="6"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="20"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
       <c r="B30" s="6"/>
       <c r="C30" s="15"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
       <c r="B31" s="6"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
       <c r="B32" s="6"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="22"/>
       <c r="B33" s="6"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>7</v>
@@ -2353,8 +2387,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="15"/>
@@ -2363,39 +2397,39 @@
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="20"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="20"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>7</v>
@@ -2432,21 +2466,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7EF1C7-726B-3A43-A014-A75014D213D7}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="20">
         <v>43605</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2454,7 +2488,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2462,7 +2496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2470,7 +2504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2478,39 +2512,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>43606</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>43607</v>
       </c>
     </row>

</xml_diff>